<commit_message>
Updated task for rescaling heatmap as it is complete, AWS deploy is now priority 5
</commit_message>
<xml_diff>
--- a/LandMaverickBacklog.xlsx
+++ b/LandMaverickBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ke416bo/Sites/LandMaverick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20F96FBB-D146-2746-8F14-E6F18B4CE341}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA1C56FD-12F3-5743-9F56-BB6017D68ACD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{75249D5A-09EB-3C4E-AF0D-916F207E8AC2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -142,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -166,6 +166,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +484,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,15 +570,24 @@
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated tasks and added costs and estimates for backlog and completed items
</commit_message>
<xml_diff>
--- a/LandMaverickBacklog.xlsx
+++ b/LandMaverickBacklog.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ke416bo/Sites/LandMaverick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA1C56FD-12F3-5743-9F56-BB6017D68ACD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{50115217-ED13-2A4A-93BE-A1BEB2593F2C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{75249D5A-09EB-3C4E-AF0D-916F207E8AC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog with Estimates and Cost" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -93,6 +93,42 @@
   </si>
   <si>
     <t>Deploy to AWS</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Estimate Effort</t>
+  </si>
+  <si>
+    <t>Actual Effort</t>
+  </si>
+  <si>
+    <t>Add code to Git Repository</t>
+  </si>
+  <si>
+    <t>Create Backlog</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Heatmap integration into page</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Add Land Maverick Logo to Page</t>
+  </si>
+  <si>
+    <t>System Test of Phase 1</t>
+  </si>
+  <si>
+    <t>Medium/Large</t>
   </si>
 </sst>
 </file>
@@ -130,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,11 +174,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -150,23 +201,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BA9423-DD41-904C-82D3-838CAE69E832}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,102 +559,308 @@
     <col min="5" max="5" width="78.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="11">
+        <v>4</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="11">
+        <v>3</v>
+      </c>
+      <c r="H2" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="14">
+        <v>11</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="14">
+        <v>16</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14">
+        <v>12</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="14">
+        <v>24</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="11">
+        <v>3</v>
+      </c>
+      <c r="H6" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="16">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="11">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="11">
+        <v>4</v>
+      </c>
+      <c r="H9" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="11">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="11">
+        <v>4</v>
+      </c>
+      <c r="H10" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="11">
+        <v>16</v>
+      </c>
+      <c r="H11" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="11">
+        <v>3</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="11">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="11">
+        <v>8</v>
+      </c>
+      <c r="H13" s="11">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>16</v>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="H15" s="6">
+        <f>SUM(H2:H13)</f>
+        <v>40</v>
+      </c>
+      <c r="I15" s="6">
+        <f>SUM(75*H15)</f>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>